<commit_message>
Fixing diode and MIM issues for models
</commit_message>
<xml_diff>
--- a/models/ngspice/testing/180MCU_SPICE_DATA/Diode/diode_nd2ps_03v3_cv.nl_out.xlsx
+++ b/models/ngspice/testing/180MCU_SPICE_DATA/Diode/diode_nd2ps_03v3_cv.nl_out.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="15">
   <si>
-    <t xml:space="preserve">W (um)</t>
+    <t xml:space="preserve">Area</t>
   </si>
   <si>
-    <t xml:space="preserve">L (um)</t>
+    <t xml:space="preserve">Pj</t>
   </si>
   <si>
     <t xml:space="preserve">corners</t>
@@ -113,13 +113,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -268,7 +268,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -304,7 +304,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -345,7 +345,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -366,6 +366,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -520,7 +525,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -541,6 +546,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -695,7 +705,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -716,6 +726,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -839,11 +854,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="92312661"/>
-        <c:axId val="43813855"/>
+        <c:axId val="64061275"/>
+        <c:axId val="48300293"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92312661"/>
+        <c:axId val="64061275"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -902,7 +917,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -933,13 +948,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43813855"/>
+        <c:crossAx val="48300293"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43813855"/>
+        <c:axId val="48300293"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -998,7 +1013,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -1029,7 +1044,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92312661"/>
+        <c:crossAx val="64061275"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1038,7 +1053,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -1050,7 +1065,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -1086,7 +1101,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1122,7 +1137,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -1163,7 +1178,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1184,6 +1199,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -1338,7 +1358,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1359,6 +1379,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -1513,7 +1538,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1534,6 +1559,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -1657,11 +1687,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83115358"/>
-        <c:axId val="22045013"/>
+        <c:axId val="62221238"/>
+        <c:axId val="98931457"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83115358"/>
+        <c:axId val="62221238"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -1720,7 +1750,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -1751,13 +1781,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22045013"/>
+        <c:crossAx val="98931457"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22045013"/>
+        <c:axId val="98931457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -1816,7 +1846,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -1847,7 +1877,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83115358"/>
+        <c:crossAx val="62221238"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1856,7 +1886,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -1868,7 +1898,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -1904,7 +1934,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1940,7 +1970,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -1981,7 +2011,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2002,6 +2032,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -2156,7 +2191,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2177,6 +2212,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -2331,7 +2371,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2352,6 +2392,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -2475,11 +2520,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="32850349"/>
-        <c:axId val="57161301"/>
+        <c:axId val="14212671"/>
+        <c:axId val="34837744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32850349"/>
+        <c:axId val="14212671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -2538,7 +2583,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -2569,13 +2614,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57161301"/>
+        <c:crossAx val="34837744"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57161301"/>
+        <c:axId val="34837744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130"/>
@@ -2634,7 +2679,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -2665,7 +2710,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32850349"/>
+        <c:crossAx val="14212671"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -2674,7 +2719,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -2686,7 +2731,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -2722,7 +2767,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2758,7 +2803,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -2799,7 +2844,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2820,6 +2865,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -2974,7 +3024,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2995,6 +3045,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -3149,7 +3204,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -3170,6 +3225,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -3293,11 +3353,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53340162"/>
-        <c:axId val="96244732"/>
+        <c:axId val="22184242"/>
+        <c:axId val="52443344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53340162"/>
+        <c:axId val="22184242"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -3356,7 +3416,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -3387,13 +3447,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96244732"/>
+        <c:crossAx val="52443344"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96244732"/>
+        <c:axId val="52443344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -3452,7 +3512,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -3483,7 +3543,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53340162"/>
+        <c:crossAx val="22184242"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -3492,7 +3552,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -3504,7 +3564,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -3540,7 +3600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3576,7 +3636,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -3617,7 +3677,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -3638,6 +3698,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -3792,7 +3857,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -3813,6 +3878,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -3967,7 +4037,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -3988,6 +4058,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -4111,11 +4186,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="38257484"/>
-        <c:axId val="44600544"/>
+        <c:axId val="64310539"/>
+        <c:axId val="87198304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38257484"/>
+        <c:axId val="64310539"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4174,7 +4249,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -4205,13 +4280,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44600544"/>
+        <c:crossAx val="87198304"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44600544"/>
+        <c:axId val="87198304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -4270,7 +4345,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -4301,7 +4376,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38257484"/>
+        <c:crossAx val="64310539"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -4310,7 +4385,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -4322,7 +4397,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -4358,7 +4433,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4394,7 +4469,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -4435,7 +4510,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -4456,6 +4531,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -4610,7 +4690,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -4631,6 +4711,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -4785,7 +4870,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -4806,6 +4891,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -4929,11 +5019,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48447534"/>
-        <c:axId val="37366867"/>
+        <c:axId val="31385766"/>
+        <c:axId val="69923060"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48447534"/>
+        <c:axId val="31385766"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4992,7 +5082,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -5023,13 +5113,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37366867"/>
+        <c:crossAx val="69923060"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37366867"/>
+        <c:axId val="69923060"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="75"/>
@@ -5088,7 +5178,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -5119,7 +5209,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48447534"/>
+        <c:crossAx val="31385766"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -5128,7 +5218,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -5140,7 +5230,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -5176,7 +5266,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5212,7 +5302,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -5253,7 +5343,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -5274,6 +5364,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -5428,7 +5523,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -5449,6 +5544,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -5603,7 +5703,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -5624,6 +5724,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -5747,11 +5852,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="49953859"/>
-        <c:axId val="72408236"/>
+        <c:axId val="51810356"/>
+        <c:axId val="65658805"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49953859"/>
+        <c:axId val="51810356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -5810,7 +5915,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -5841,13 +5946,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72408236"/>
+        <c:crossAx val="65658805"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72408236"/>
+        <c:axId val="65658805"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -5906,7 +6011,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -5937,7 +6042,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49953859"/>
+        <c:crossAx val="51810356"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -5946,7 +6051,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -5958,7 +6063,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -5994,7 +6099,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6030,7 +6135,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -6071,7 +6176,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -6092,6 +6197,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -6246,7 +6356,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -6267,6 +6377,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -6421,7 +6536,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -6442,6 +6557,11 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -6565,11 +6685,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="97855340"/>
-        <c:axId val="45756033"/>
+        <c:axId val="49786161"/>
+        <c:axId val="33626076"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97855340"/>
+        <c:axId val="49786161"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -6628,7 +6748,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -6659,13 +6779,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45756033"/>
+        <c:crossAx val="33626076"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45756033"/>
+        <c:axId val="33626076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -6724,7 +6844,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -6755,7 +6875,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97855340"/>
+        <c:crossAx val="49786161"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6763,7 +6883,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -6775,7 +6895,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -6822,9 +6942,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>276480</xdr:colOff>
+      <xdr:colOff>276120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6832,8 +6952,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17334000" y="10159920"/>
-        <a:ext cx="8951760" cy="4095360"/>
+        <a:off x="17334000" y="10160280"/>
+        <a:ext cx="8951760" cy="4095000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6852,9 +6972,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6862,8 +6982,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26286120" y="10159920"/>
-        <a:ext cx="8952120" cy="4095360"/>
+        <a:off x="26286480" y="10160280"/>
+        <a:ext cx="8951400" cy="4095000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6882,9 +7002,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>276480</xdr:colOff>
+      <xdr:colOff>276120</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6892,8 +7012,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17334000" y="14255640"/>
-        <a:ext cx="8951760" cy="4095360"/>
+        <a:off x="17334000" y="14256000"/>
+        <a:ext cx="8951760" cy="4094640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6912,9 +7032,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6922,8 +7042,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26286120" y="14255640"/>
-        <a:ext cx="8952120" cy="4095360"/>
+        <a:off x="26286480" y="14256000"/>
+        <a:ext cx="8951400" cy="4094640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6942,9 +7062,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>276480</xdr:colOff>
+      <xdr:colOff>276120</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6953,7 +7073,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="17334000" y="18351360"/>
-        <a:ext cx="8951760" cy="4095360"/>
+        <a:ext cx="8951760" cy="4095000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6972,9 +7092,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6982,8 +7102,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26286120" y="18351360"/>
-        <a:ext cx="8952120" cy="4095360"/>
+        <a:off x="26286480" y="18351360"/>
+        <a:ext cx="8951400" cy="4095000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7002,9 +7122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>276480</xdr:colOff>
+      <xdr:colOff>276120</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7032,9 +7152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7042,8 +7162,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26286120" y="22447080"/>
-        <a:ext cx="8952120" cy="4095360"/>
+        <a:off x="26286480" y="22447080"/>
+        <a:ext cx="8951400" cy="4095360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7064,7 +7184,7 @@
   <dimension ref="A1:BP65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B9"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10236,8 +10356,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>